<commit_message>
Ensayo exitoso conexion BD
</commit_message>
<xml_diff>
--- a/src/test/resources/resultados y pronosticos para chequear puntajes.xlsx
+++ b/src/test/resources/resultados y pronosticos para chequear puntajes.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="resultados" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="pronosticos para guardar como c" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="41">
   <si>
     <t xml:space="preserve">Fase - id</t>
   </si>
@@ -109,42 +110,56 @@
     <t xml:space="preserve">Gana 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Mariana</t>
+    <t xml:space="preserve">X acierta todos en cada ronda menos uno (hay 2 rondas)</t>
   </si>
   <si>
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">Pedro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mariana 4 puntos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 aciertos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedro 2 puntos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 aciertos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no se usa Fase 2 porque no se cargaron pronosticos para fase 2</t>
+    <t xml:space="preserve">X acierta todos en cada ronda (hay 2 rondas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y acierta todos en una FASE menos uno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y acierta todos en una FASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X acierta todos en una FASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aciertos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puntos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suplem. x ronda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supl. x fase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUNTAJE TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No se usa Fase 2 de resultados porque no se cargaron pronosticos para fase 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,6 +175,29 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0008FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -216,7 +254,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,6 +264,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -244,7 +298,7 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0008FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
@@ -292,7 +346,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -306,22 +360,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="21.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.49"/>
@@ -878,7 +932,7 @@
       <c r="G16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J16" s="1"/>
@@ -995,7 +1049,8 @@
       <c r="G20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="2"/>
+      <c r="J20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K20" s="0" t="n">
@@ -1024,10 +1079,9 @@
       <c r="G21" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="K21" s="0" t="n">
         <v>7</v>
       </c>
@@ -1054,8 +1108,7 @@
       <c r="G22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="0" t="s">
+      <c r="H22" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K22" s="0" t="n">
@@ -1084,8 +1137,7 @@
       <c r="G23" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="J23" s="0" t="s">
+      <c r="H23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K23" s="0" t="n">
@@ -1114,10 +1166,9 @@
       <c r="G24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="K24" s="0" t="n">
         <v>2</v>
       </c>
@@ -1144,8 +1195,7 @@
       <c r="G25" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="0" t="s">
+      <c r="I25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K25" s="0" t="n">
@@ -1203,10 +1253,9 @@
       <c r="G27" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="K27" s="0" t="n">
         <v>3</v>
       </c>
@@ -1262,10 +1311,9 @@
       <c r="G29" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H29" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I29" s="2"/>
+      <c r="I29" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="K29" s="0" t="n">
         <v>7</v>
       </c>
@@ -1292,8 +1340,7 @@
       <c r="G30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="J30" s="0" t="s">
+      <c r="H30" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K30" s="0" t="n">
@@ -1322,33 +1369,575 @@
       <c r="G31" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="0" t="s">
+      <c r="H31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K31" s="0" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="0" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="C32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H33" s="0"/>
+      <c r="I33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" s="0" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="0" t="s">
+      <c r="C40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="C47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="0" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="0" t="s">
+      <c r="F49" s="0" t="s">
         <v>36</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I50" s="6" t="n">
+        <f aca="false">SUM(F50:H50)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I51" s="6" t="n">
+        <f aca="false">SUM(F51:H51)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" s="6" t="n">
+        <f aca="false">SUM(F52:H52)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" s="6" t="n">
+        <f aca="false">SUM(F53:H53)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1360,4 +1949,994 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="J6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>